<commit_message>
change in upload sheet
</commit_message>
<xml_diff>
--- a/src/main/resources/ProjectDescription.xlsx
+++ b/src/main/resources/ProjectDescription.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Srividya\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajithkv\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="PSK_DESC" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>Serial Number</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>Alias Description</t>
+  </si>
+  <si>
+    <t>Quanity</t>
+  </si>
+  <si>
+    <t>Metric</t>
   </si>
   <si>
     <t>Base Description</t>
@@ -429,20 +435,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F498"/>
+  <dimension ref="A1:F495"/>
   <sheetViews>
-    <sheetView topLeftCell="A493" workbookViewId="0">
-      <selection sqref="A1:F498"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="31.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" customWidth="1"/>
-    <col min="5" max="5" width="33.28515625" customWidth="1"/>
-    <col min="6" max="6" width="27.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.85546875" customWidth="1"/>
+    <col min="6" max="6" width="44.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -4417,39 +4423,15 @@
       <c r="E495" s="2"/>
       <c r="F495" s="2"/>
     </row>
-    <row r="496" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A496" s="2"/>
-      <c r="B496" s="2"/>
-      <c r="C496" s="2"/>
-      <c r="D496" s="2"/>
-      <c r="E496" s="2"/>
-      <c r="F496" s="2"/>
-    </row>
-    <row r="497" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A497" s="2"/>
-      <c r="B497" s="2"/>
-      <c r="C497" s="2"/>
-      <c r="D497" s="2"/>
-      <c r="E497" s="2"/>
-      <c r="F497" s="2"/>
-    </row>
-    <row r="498" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A498" s="2"/>
-      <c r="B498" s="2"/>
-      <c r="C498" s="2"/>
-      <c r="D498" s="2"/>
-      <c r="E498" s="2"/>
-      <c r="F498" s="2"/>
-    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B498">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B495">
       <formula1>"Main Work,Electrical,Plumbing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D498">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D495">
       <formula1>"BAG,CFT,CUM (m3),EACH,KG,LIT,MT,NOS,QUINTAL,RFT,RM,SQFT,SQM,UNIT"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C498">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C495">
       <formula1>0.01</formula1>
       <formula2>200000</formula2>
     </dataValidation>
@@ -4461,10 +4443,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G498"/>
+  <dimension ref="A1:G496"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4473,8 +4455,9 @@
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
     <col min="4" max="4" width="28.5703125" customWidth="1"/>
-    <col min="5" max="6" width="33.28515625" customWidth="1"/>
-    <col min="7" max="7" width="27.5703125" customWidth="1"/>
+    <col min="5" max="5" width="33.28515625" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" customWidth="1"/>
+    <col min="7" max="7" width="43.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -4485,10 +4468,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -4497,7 +4480,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -8955,34 +8938,16 @@
       <c r="F496" s="2"/>
       <c r="G496" s="2"/>
     </row>
-    <row r="497" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A497" s="2"/>
-      <c r="B497" s="2"/>
-      <c r="C497" s="2"/>
-      <c r="D497" s="2"/>
-      <c r="E497" s="2"/>
-      <c r="F497" s="2"/>
-      <c r="G497" s="2"/>
-    </row>
-    <row r="498" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A498" s="2"/>
-      <c r="B498" s="2"/>
-      <c r="C498" s="2"/>
-      <c r="D498" s="2"/>
-      <c r="E498" s="2"/>
-      <c r="F498" s="2"/>
-      <c r="G498" s="2"/>
-    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C498">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C496">
       <formula1>0.01</formula1>
       <formula2>200000</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D498">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D496">
       <formula1>"BAG,CFT,CUM (m3),EACH,KG,LIT,MT,NOS,QUINTAL,RFT,RM,SQFT,SQM,UNIT"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B498">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B496">
       <formula1>"Main Work,Electrical,Plumbing"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Production Change - Added Hours to excel template metric - Sriram.
</commit_message>
<xml_diff>
--- a/src/main/resources/ProjectDescription.xlsx
+++ b/src/main/resources/ProjectDescription.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajithkv\Desktop\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Srividya\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -430,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G496"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4913,12 +4913,12 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B495">
       <formula1>"Main Work,Electrical,Plumbing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D495">
-      <formula1>"BAG,CFT,CUM (m3),EACH,KG,LIT,MT,NOS,QUINTAL,RFT,RM,SQFT,SQM,UNIT"</formula1>
-    </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C495">
       <formula1>0.01</formula1>
       <formula2>200000</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D495">
+      <formula1>"BAG,CFT,CUM (m3),EACH,Hours,KG,LIT,MT,NOS,QUINTAL,RFT,RM,SQFT,SQM,UNIT"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>